<commit_message>
modified:   app/Http/Controllers/Penerimaan.php 	modified:   public/file_excel/ContohUploadLegalitas.xlsx 	modified:   resources/views/products/02_penerimaan/legalitasEdit.blade.php 	modified:   routes/web.php
</commit_message>
<xml_diff>
--- a/public/file_excel/ContohUploadLegalitas.xlsx
+++ b/public/file_excel/ContohUploadLegalitas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerjaan\pintex-ehrd\public\file_excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shannon\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC3E6121-C367-41DA-BCDE-3843B919E95E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{125AE8C4-AB4B-4C25-8416-553887AD59E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CCEEB5C7-24C0-425E-A268-49AAC839D68C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCEEB5C7-24C0-425E-A268-49AAC839D68C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>PERJANJIAN</t>
   </si>
@@ -106,6 +106,27 @@
   </si>
   <si>
     <t>NAMA KARYAWAN</t>
+  </si>
+  <si>
+    <t>HERLAMBANG YUDHA P</t>
+  </si>
+  <si>
+    <t>*JENIS</t>
+  </si>
+  <si>
+    <t>BASIC</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>INTERNAL</t>
+  </si>
+  <si>
+    <t>OL-001</t>
+  </si>
+  <si>
+    <t>YUDHA</t>
   </si>
 </sst>
 </file>
@@ -130,7 +151,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,13 +160,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -177,10 +210,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,126 +537,189 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
-    <col min="6" max="8" width="16.5703125" customWidth="1"/>
-    <col min="17" max="17" width="21.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.140625" style="1"/>
-    <col min="19" max="19" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.44140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2">
+        <v>122043</v>
+      </c>
+      <c r="E2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="3">
+        <v>45432</v>
+      </c>
+      <c r="G2" s="3">
+        <v>45797</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="R2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q3" s="1" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="3">
+        <v>45432</v>
+      </c>
+      <c r="G3" s="3">
+        <v>45797</v>
+      </c>
+      <c r="H3">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="S3" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q4" s="1" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q5" s="1" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="Q6" s="1" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="Q6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S7" s="1" t="s">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S7" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S8" s="1" t="s">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S8" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S9" s="1" t="s">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S9" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S10" s="1" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S10" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S11" s="1" t="s">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S12" s="1" t="s">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S12" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S13" s="1" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S13" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="S14" s="1" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="S14" s="6" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>